<commit_message>
MBtech and Brunel, Excel update
</commit_message>
<xml_diff>
--- a/Personal/Anschreiben & Stellen/Übersicht.xlsx
+++ b/Personal/Anschreiben & Stellen/Übersicht.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="60">
   <si>
     <t>Firma</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -174,6 +174,78 @@
   <si>
     <t>14.09.15</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>17.09 Tel-Interview</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gespräch am 22.09</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10.09 Inteview</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Im Lauf</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Abgesagt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Siemens</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Siemens Graduate Program – Digital Factory Division – Business Development –</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> Beijing</t>
+  </si>
+  <si>
+    <t>Siemens Graduate Program–Siemens Wind Power Blades –Production Management-Shanghai</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shanghai</t>
+  </si>
+  <si>
+    <t>19.09.15</t>
+  </si>
+  <si>
+    <t>19.09.15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Anmerkung</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>yingjiesheng.com-han_tiger7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bosch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Algorithm Development</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shanghai</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>51job han_tiger7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t> Software Engineer (Radar) 软件工程师 （雷达）(汽车底盘控制 )</t>
   </si>
 </sst>
 </file>
@@ -181,9 +253,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="178" formatCode="[$-407]d\.\ mmm\ yy;@"/>
+    <numFmt numFmtId="176" formatCode="[$-407]d\.\ mmm\ yy;@"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -210,6 +282,19 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF124771"/>
+      <name val="Arial, Helvetica, sans-serif;宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="2">
@@ -275,7 +360,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -300,10 +385,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -601,10 +692,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -612,9 +703,10 @@
     <col min="1" max="1" width="20.75" customWidth="1"/>
     <col min="2" max="2" width="42.125" customWidth="1"/>
     <col min="3" max="3" width="29.75" style="4" customWidth="1"/>
-    <col min="4" max="4" width="37.125" style="9" customWidth="1"/>
-    <col min="5" max="5" width="21.875" customWidth="1"/>
-    <col min="6" max="6" width="14.75" customWidth="1"/>
+    <col min="4" max="4" width="21.5" style="9" customWidth="1"/>
+    <col min="5" max="5" width="21.875" style="4" customWidth="1"/>
+    <col min="6" max="6" width="21.25" customWidth="1"/>
+    <col min="7" max="7" width="21.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="4" customFormat="1" ht="15" thickTop="1" thickBot="1">
@@ -636,9 +728,11 @@
       <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3"/>
-    </row>
-    <row r="2" spans="1:7" ht="20.100000000000001" customHeight="1" thickTop="1">
+      <c r="G1" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="54.75" customHeight="1" thickTop="1">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -693,6 +787,12 @@
       <c r="D5" s="9" t="s">
         <v>16</v>
       </c>
+      <c r="E5" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F5" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="6" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A6" t="s">
@@ -763,6 +863,12 @@
       <c r="D10" s="9" t="s">
         <v>29</v>
       </c>
+      <c r="E10" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="11" spans="1:7" ht="43.5" customHeight="1">
       <c r="A11" t="s">
@@ -777,6 +883,12 @@
       <c r="D11" s="9" t="s">
         <v>12</v>
       </c>
+      <c r="E11" s="4">
+        <v>18.09</v>
+      </c>
+      <c r="F11" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="12" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A12" t="s">
@@ -792,7 +904,59 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="20.100000000000001" customHeight="1"/>
+    <row r="13" spans="1:7" ht="29.25" customHeight="1">
+      <c r="A13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="G13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="22.5">
+      <c r="A14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="G15" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="B16" s="11" t="s">
+        <v>59</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:F13">
     <sortCondition descending="1" ref="D1"/>

</xml_diff>